<commit_message>
feat: lab6 aisd & modification for lab5
</commit_message>
<xml_diff>
--- a/sem2/aisd-lab/src/lab5/aisd_wykresy_lista5.xlsx
+++ b/sem2/aisd-lab/src/lab5/aisd_wykresy_lista5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projekty\pwr-repo\sem2\aisd-lab\src\lab5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F673093-8857-4DAD-8986-6CDED94F347B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F259D76C-C83A-4A33-BA34-544B792B34DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="3" xr2:uid="{C7128112-AAFE-497F-80CF-4D7C130D65FB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="2" xr2:uid="{C7128112-AAFE-497F-80CF-4D7C130D65FB}"/>
   </bookViews>
   <sheets>
     <sheet name="OrderedGenerator" sheetId="1" r:id="rId1"/>
@@ -35911,7 +35911,7 @@
   </sheetPr>
   <dimension ref="A1:AC137"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="49" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H128" sqref="H128"/>
     </sheetView>
   </sheetViews>
@@ -38918,7 +38918,7 @@
   </sheetPr>
   <dimension ref="A1:AC137"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" zoomScale="67" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="50" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="A118" sqref="A118:G137"/>
     </sheetView>
   </sheetViews>
@@ -41925,7 +41925,7 @@
   </sheetPr>
   <dimension ref="A1:AC137"/>
   <sheetViews>
-    <sheetView topLeftCell="A104" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A118" sqref="A118:G137"/>
     </sheetView>
   </sheetViews>
@@ -44932,7 +44932,7 @@
   </sheetPr>
   <dimension ref="A1:AC137"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="56" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A118" sqref="A118:G137"/>
     </sheetView>
   </sheetViews>

</xml_diff>